<commit_message>
major rebuild. Eliminate mixed case variables (excepting In/Out). Clean documentation
</commit_message>
<xml_diff>
--- a/data-raw/res2A_focus.xlsx
+++ b/data-raw/res2A_focus.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zurp/Dropbox (Personal)/diss/analy/vid-coding/res2A-focus-hand. in prog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zurp/Dropbox (Personal)/diss/analy/vid-coding/res2A-focus. done/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12080" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mdg_20180104" sheetId="4" r:id="rId1"/>
     <sheet name="slg_20180104" sheetId="5" r:id="rId2"/>
+    <sheet name="slg_20180212" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="159">
   <si>
     <t>Coder</t>
   </si>
@@ -388,6 +389,123 @@
   </si>
   <si>
     <t>14:33</t>
+  </si>
+  <si>
+    <t>01:47</t>
+  </si>
+  <si>
+    <t>03:49</t>
+  </si>
+  <si>
+    <t>05:12</t>
+  </si>
+  <si>
+    <t>05:22</t>
+  </si>
+  <si>
+    <t>07:15</t>
+  </si>
+  <si>
+    <t>07:53</t>
+  </si>
+  <si>
+    <t>09:20</t>
+  </si>
+  <si>
+    <t>10:24</t>
+  </si>
+  <si>
+    <t>10:35</t>
+  </si>
+  <si>
+    <t>11:55</t>
+  </si>
+  <si>
+    <t>12:45</t>
+  </si>
+  <si>
+    <t>12:48</t>
+  </si>
+  <si>
+    <t>13:45</t>
+  </si>
+  <si>
+    <t>14:25</t>
+  </si>
+  <si>
+    <t>14:54</t>
+  </si>
+  <si>
+    <t>15:24</t>
+  </si>
+  <si>
+    <t>16:17</t>
+  </si>
+  <si>
+    <t>16:19</t>
+  </si>
+  <si>
+    <t>17:46</t>
+  </si>
+  <si>
+    <t>17:48</t>
+  </si>
+  <si>
+    <t>17:56</t>
+  </si>
+  <si>
+    <t>20:03</t>
+  </si>
+  <si>
+    <t>20:12</t>
+  </si>
+  <si>
+    <t>20:46</t>
+  </si>
+  <si>
+    <t>00:48</t>
+  </si>
+  <si>
+    <t>03:09</t>
+  </si>
+  <si>
+    <t>03:36</t>
+  </si>
+  <si>
+    <t>05:42</t>
+  </si>
+  <si>
+    <t>06:49</t>
+  </si>
+  <si>
+    <t>07:07</t>
+  </si>
+  <si>
+    <t>10:22</t>
+  </si>
+  <si>
+    <t>10:46</t>
+  </si>
+  <si>
+    <t>11:02</t>
+  </si>
+  <si>
+    <t>11:16</t>
+  </si>
+  <si>
+    <t>11:35</t>
+  </si>
+  <si>
+    <t>11:48</t>
+  </si>
+  <si>
+    <t>13:17</t>
+  </si>
+  <si>
+    <t>16:54</t>
+  </si>
+  <si>
+    <t>18:40</t>
   </si>
 </sst>
 </file>
@@ -993,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE10D47-70A0-574D-B2E3-ED3263117924}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2201,7 @@
         <v>84</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2369,8 +2487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A5F639-D40E-E244-AF2B-FF9F367AD031}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A42"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3148,5 +3266,1341 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC970EC-73CB-054D-A0F4-06C3F4D72DE9}">
+  <dimension ref="A1:E100"/>
+  <sheetViews>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>